<commit_message>
add survey questions for learning outcome
</commit_message>
<xml_diff>
--- a/data/Survey_data.xlsx
+++ b/data/Survey_data.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/MFF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/MFF/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9EE88A9-E2DE-9440-ABCA-837CA3DF3462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437D1E80-C5C7-A842-A83B-8B04F7922B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{AB8B5367-E5AA-D647-B626-0E1BAE1383D0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Survey_Football_Player" sheetId="1" r:id="rId1"/>
+    <sheet name="Survey_Coach" sheetId="2" r:id="rId2"/>
+    <sheet name="Survey_Chef_Cook" sheetId="3" r:id="rId3"/>
+    <sheet name="Survey_Management" sheetId="4" r:id="rId4"/>
+    <sheet name="Survey_Medical" sheetId="5" r:id="rId5"/>
+    <sheet name="Survey_Sports_Science" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,9 +40,279 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+  <si>
+    <t>Upper bound</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower bound </t>
+  </si>
+  <si>
+    <t>Very important             5</t>
+  </si>
+  <si>
+    <t>Learning_outcome</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Never                                  1</t>
+  </si>
+  <si>
+    <t>Always                          5</t>
+  </si>
+  <si>
+    <t>Very well                      5</t>
+  </si>
+  <si>
+    <t>3. How well do MFF players know the food groups?</t>
+  </si>
+  <si>
+    <t>2. How often do MFF players take care of their diet?</t>
+  </si>
+  <si>
+    <t>1. How important is nutrition for  football players at MFF?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q1?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q2?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q3?</t>
+  </si>
+  <si>
+    <t>4. How well do MFF players know nutrients and their food sources?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q4?</t>
+  </si>
+  <si>
+    <t>5. How well do MFF players know healthy plate and healthy eating?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q5?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. How well do MFF players know nutrient and fluid requirements for football player? </t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q6?</t>
+  </si>
+  <si>
+    <t>7. How well do MFF players know how to calculate protein-energy/ fluid requirements?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q7?</t>
+  </si>
+  <si>
+    <t>8. How well do MFF players plan their own meals/ diet?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q8?</t>
+  </si>
+  <si>
+    <t>9. Are MFF players familiar with food exchange list?</t>
+  </si>
+  <si>
+    <t>Very familiar                5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q9?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q10?</t>
+  </si>
+  <si>
+    <t>11. Are MFF players interested in advanced nutrition training?</t>
+  </si>
+  <si>
+    <t>Very interested             5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q11?</t>
+  </si>
+  <si>
+    <t>12. Will MFF players be motivated to apply the knowledge after training?</t>
+  </si>
+  <si>
+    <t>Very motivated.            5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q12?</t>
+  </si>
+  <si>
+    <t>Very relevant/useful    5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q13?</t>
+  </si>
+  <si>
+    <t>Very unimportant.              1</t>
+  </si>
+  <si>
+    <t>Very poorly                         1</t>
+  </si>
+  <si>
+    <t>Very incomprehensible      1</t>
+  </si>
+  <si>
+    <t>Very irrelevant/useless     1</t>
+  </si>
+  <si>
+    <t>Very uninterested              1</t>
+  </si>
+  <si>
+    <t>Very unmotivated              1</t>
+  </si>
+  <si>
+    <t>Very comprehensible   5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q14?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q15?</t>
+  </si>
+  <si>
+    <t>Very difficult                      1</t>
+  </si>
+  <si>
+    <t>Very easy                      5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q16?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. How often do MFF players follow a diet plan? </t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q17?</t>
+  </si>
+  <si>
+    <t>Please see the details of the two interventions and accompanying resources before answering Q 11 to 16.</t>
+  </si>
+  <si>
+    <t>18. After the training, how likely will MFF players apply the knowledge and eat according to guidelines without being prompted?</t>
+  </si>
+  <si>
+    <t>Very unlikely                      1</t>
+  </si>
+  <si>
+    <t>Very likely                     5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q18?</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q19?</t>
+  </si>
+  <si>
+    <t>Very bad                             1</t>
+  </si>
+  <si>
+    <t>Very good                     5</t>
+  </si>
+  <si>
+    <t>What percentage of football players at MFF would rate 4 or 5 for Q20?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17. How well can MFF players solve mathematic problems using unitary method? </t>
+  </si>
+  <si>
+    <t>Very unfamiliar                  1</t>
+  </si>
+  <si>
+    <t>19. How likely will MFF players find time to study the nutrition notes and practice the calculations?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">14. After reviewing the provided resources, please rate the clarity and comprehensibility of the initial four chapters of the nutrition guide. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Think for all MFF players)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">15. After reviewing the provided resources, please rate the clarity and comprehensibility of the final two chapters of the nutrition guide. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Think for all MFF players)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">13. After reviewing the provided resources, please rate the relevancy/usefulness of the learning materials. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Think for all MFF players)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">16. After reviewing the provided resources, please rate the ease of use for the materials provided, including food exchange list, food tray with designated spaces, and cup/bottle.  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Think for all MFF players)</t>
+    </r>
+  </si>
+  <si>
+    <t>20. What do MFF players think about the current training venue?</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,16 +320,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +365,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,9 +705,608 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E66099-BEB7-0F48-9BBB-E2C4027784D4}">
+  <dimension ref="A1:M44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="174.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="9" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="4.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>57</v>
+      </c>
+      <c r="K38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42" t="s">
+        <v>61</v>
+      </c>
+      <c r="K42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B61A228-35C8-E64C-99C5-9584F008DE00}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A0603F-B030-014F-AFD2-3FA4DA665280}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46B4141-8614-1F48-97BA-62DA8098979A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E75A960-0BD4-C749-8EBD-6A78E25B9FD7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13CCE91-C373-E747-BDE0-7FC133416E8E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
add value to survey data
</commit_message>
<xml_diff>
--- a/data/Survey_data.xlsx
+++ b/data/Survey_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/MFF/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437D1E80-C5C7-A842-A83B-8B04F7922B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC24E70-00E2-AD45-A6FA-DFEA603A07C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{AB8B5367-E5AA-D647-B626-0E1BAE1383D0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Survey_Medical" sheetId="5" r:id="rId5"/>
     <sheet name="Survey_Sports_Science" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -378,19 +378,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E66099-BEB7-0F48-9BBB-E2C4027784D4}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,7 +715,7 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="174.83203125" customWidth="1"/>
+    <col min="4" max="4" width="106.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="9" max="9" width="20.5" customWidth="1"/>
@@ -739,14 +738,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
@@ -761,6 +760,12 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
@@ -782,8 +787,20 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
+      <c r="L2">
+        <v>0.7</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
@@ -805,8 +822,20 @@
       <c r="K4" t="s">
         <v>16</v>
       </c>
+      <c r="L4">
+        <v>0.3</v>
+      </c>
+      <c r="M4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -828,8 +857,20 @@
       <c r="K6" t="s">
         <v>17</v>
       </c>
+      <c r="L6">
+        <v>0.7</v>
+      </c>
+      <c r="M6">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
@@ -851,8 +892,20 @@
       <c r="K8" t="s">
         <v>19</v>
       </c>
+      <c r="L8">
+        <v>0.3</v>
+      </c>
+      <c r="M8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
@@ -874,8 +927,20 @@
       <c r="K10" t="s">
         <v>21</v>
       </c>
+      <c r="L10">
+        <v>0.3</v>
+      </c>
+      <c r="M10">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
@@ -897,8 +962,20 @@
       <c r="K12" t="s">
         <v>23</v>
       </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
@@ -920,8 +997,20 @@
       <c r="K14" t="s">
         <v>25</v>
       </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
@@ -943,8 +1032,20 @@
       <c r="K16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
       <c r="D18" t="s">
         <v>28</v>
       </c>
@@ -966,8 +1067,20 @@
       <c r="K18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
       <c r="D20" t="s">
         <v>52</v>
       </c>
@@ -989,16 +1102,25 @@
       <c r="K20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="7" t="s">
+      <c r="L20">
+        <v>0.1</v>
+      </c>
+      <c r="M20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
       <c r="D24" t="s">
         <v>32</v>
       </c>
@@ -1020,8 +1142,20 @@
       <c r="K24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>0.7</v>
+      </c>
+      <c r="M24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
       <c r="D26" t="s">
         <v>35</v>
       </c>
@@ -1043,8 +1177,20 @@
       <c r="K26" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>0.7</v>
+      </c>
+      <c r="M26">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
       <c r="D28" t="s">
         <v>68</v>
       </c>
@@ -1066,8 +1212,20 @@
       <c r="K28" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>0.7</v>
+      </c>
+      <c r="M28">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
       <c r="D30" t="s">
         <v>66</v>
       </c>
@@ -1089,8 +1247,20 @@
       <c r="K30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>0.7</v>
+      </c>
+      <c r="M30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
       <c r="D32" t="s">
         <v>67</v>
       </c>
@@ -1112,8 +1282,20 @@
       <c r="K32" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>0.3</v>
+      </c>
+      <c r="M32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
       <c r="D34" t="s">
         <v>69</v>
       </c>
@@ -1135,8 +1317,20 @@
       <c r="K34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>0.3</v>
+      </c>
+      <c r="M34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
       <c r="D36" t="s">
         <v>63</v>
       </c>
@@ -1158,8 +1352,20 @@
       <c r="K36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>0.6</v>
+      </c>
+      <c r="M36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
       <c r="D38" t="s">
         <v>55</v>
       </c>
@@ -1181,12 +1387,21 @@
       <c r="K38" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="5" t="s">
+      <c r="L38">
+        <v>0.5</v>
+      </c>
+      <c r="M38">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
         <v>65</v>
       </c>
       <c r="E40" t="s">
@@ -1207,8 +1422,20 @@
       <c r="K40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>0.3</v>
+      </c>
+      <c r="M40">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
       <c r="D42" t="s">
         <v>70</v>
       </c>
@@ -1230,8 +1457,14 @@
       <c r="K42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="44" spans="4:11" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="L42">
+        <v>0.7</v>
+      </c>
+      <c r="M42">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:I1"/>

</xml_diff>